<commit_message>
updating daily entry with details + figure
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Crizotinib_only/Crizonitib_assay_2.xlsx
+++ b/Raw_SRB_data/Crizotinib_only/Crizonitib_assay_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,8 +345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>